<commit_message>
update Done untuk CB poin 2 sama Fatah
</commit_message>
<xml_diff>
--- a/progress fa.xlsx
+++ b/progress fa.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -458,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +589,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
petty cash dan Bank Transaction Done
</commit_message>
<xml_diff>
--- a/progress fa.xlsx
+++ b/progress fa.xlsx
@@ -458,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +613,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -621,7 +621,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ini buat CB poin 4 di kartu hutang
</commit_message>
<xml_diff>
--- a/progress fa.xlsx
+++ b/progress fa.xlsx
@@ -459,7 +459,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +605,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>